<commit_message>
Method Classification is done
</commit_message>
<xml_diff>
--- a/doc/11.07.2013 Meeting/Results.xlsx
+++ b/doc/11.07.2013 Meeting/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="63">
   <si>
     <t xml:space="preserve">method </t>
   </si>
@@ -207,6 +207,9 @@
   <si>
     <t>L2</t>
   </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
 </sst>
 </file>
 
@@ -952,11 +955,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95712768"/>
-        <c:axId val="95714304"/>
+        <c:axId val="101193984"/>
+        <c:axId val="101203968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95712768"/>
+        <c:axId val="101193984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,7 +969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95714304"/>
+        <c:crossAx val="101203968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -974,7 +977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95714304"/>
+        <c:axId val="101203968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -986,7 +989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95712768"/>
+        <c:crossAx val="101193984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2241,11 +2244,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95478912"/>
-        <c:axId val="95480448"/>
+        <c:axId val="101269504"/>
+        <c:axId val="101271040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95478912"/>
+        <c:axId val="101269504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95480448"/>
+        <c:crossAx val="101271040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2263,7 +2266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95480448"/>
+        <c:axId val="101271040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -2275,7 +2278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95478912"/>
+        <c:crossAx val="101269504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3037,11 +3040,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95658368"/>
-        <c:axId val="95659904"/>
+        <c:axId val="101313536"/>
+        <c:axId val="101327616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95658368"/>
+        <c:axId val="101313536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3051,7 +3054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95659904"/>
+        <c:crossAx val="101327616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3059,7 +3062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95659904"/>
+        <c:axId val="101327616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -3071,7 +3074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95658368"/>
+        <c:crossAx val="101313536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5453,8 +5456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5467,7 +5470,7 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
         <v>23</v>
@@ -5510,7 +5513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>